<commit_message>
Corrección plantilla iteración 7
</commit_message>
<xml_diff>
--- a/Documentos/Tareas/Iteración_7.xlsx
+++ b/Documentos/Tareas/Iteración_7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raymu\Desktop\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390E4374-FB99-4636-8051-A5951782DB40}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A07BC02-678A-436C-854A-3B33E7811A18}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2335,7 +2335,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2621,10 +2621,10 @@
     </row>
     <row r="6" spans="2:53" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>46</v>
@@ -4312,10 +4312,10 @@
     </row>
     <row r="23" spans="2:53" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D23" s="20" t="s">
         <v>46</v>
@@ -7140,6 +7140,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -7151,11 +7156,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="84" orientation="portrait" r:id="rId1"/>

</xml_diff>